<commit_message>
Updated parts list and added the dummy project folder for lab 4
</commit_message>
<xml_diff>
--- a/Piano Parts.xlsx
+++ b/Piano Parts.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27430"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10909"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Hackintosh HDD 1/CSCE 462/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEDB687F-E089-2E4E-92E9-07762E3AC84D}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="36720" windowHeight="21020" tabRatio="500"/>
+    <workbookView xWindow="80" yWindow="440" windowWidth="36720" windowHeight="21020" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="37">
   <si>
     <t>Piano Project</t>
   </si>
@@ -51,9 +57,6 @@
     <t>Parts Quantities</t>
   </si>
   <si>
-    <t>16 oz</t>
-  </si>
-  <si>
     <t>100ft</t>
   </si>
   <si>
@@ -73,9 +76,6 @@
   </si>
   <si>
     <t>100 ft</t>
-  </si>
-  <si>
-    <t>3 rolls</t>
   </si>
   <si>
     <t>Parts Unit Cost</t>
@@ -141,7 +141,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -207,6 +207,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -531,14 +539,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="143" zoomScaleNormal="143" zoomScalePageLayoutView="143" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="45.83203125" customWidth="1"/>
@@ -550,20 +558,20 @@
     <col min="9" max="9" width="13.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="H3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -571,24 +579,24 @@
         <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5">
         <v>70</v>
@@ -601,15 +609,15 @@
         <v>182</v>
       </c>
       <c r="F5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6">
         <v>70</v>
@@ -622,9 +630,9 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C7">
         <v>4</v>
@@ -637,12 +645,12 @@
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D8">
         <v>18</v>
@@ -651,21 +659,21 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D9">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="E9">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>5</v>
       </c>
@@ -679,7 +687,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>6</v>
       </c>
@@ -694,23 +702,29 @@
         <v>21.87</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>8</v>
       </c>
       <c r="C13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E14">
+        <f>E5+E6+E8+E7+E9+E10+E11</f>
+        <v>374.87</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>2</v>
       </c>
@@ -718,124 +732,182 @@
         <v>9</v>
       </c>
       <c r="D16" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
+        <v>15</v>
+      </c>
+      <c r="E16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C17">
         <v>32</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
+      <c r="D17">
+        <v>2.6</v>
+      </c>
+      <c r="E17">
+        <f>C17*D17</f>
+        <v>83.2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C18">
         <v>32</v>
       </c>
-    </row>
-    <row r="19" spans="1:3">
+      <c r="D18">
+        <v>0.4</v>
+      </c>
+      <c r="E18">
+        <f t="shared" ref="E18:E19" si="0">C18*D18</f>
+        <v>12.8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>3</v>
       </c>
       <c r="C19">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:3">
+      <c r="D19">
+        <v>16.5</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>4</v>
       </c>
       <c r="C20" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
+        <v>20</v>
+      </c>
+      <c r="D20">
+        <v>18</v>
+      </c>
+      <c r="E20">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C21" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
+        <v>16</v>
+      </c>
+      <c r="D21">
+        <v>19</v>
+      </c>
+      <c r="E21">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>5</v>
       </c>
       <c r="C22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:3">
+      <c r="D22">
+        <v>40</v>
+      </c>
+      <c r="E22">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>6</v>
       </c>
-      <c r="C23" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
+      <c r="C23">
+        <v>2</v>
+      </c>
+      <c r="D23">
+        <v>7.29</v>
+      </c>
+      <c r="E23">
+        <f>C23*D23</f>
+        <v>14.58</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>7</v>
       </c>
       <c r="C24" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>8</v>
       </c>
       <c r="C25" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E26">
+        <f>E17+E18+E19+E20+E21+E22+E23</f>
+        <v>220.58</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
-      <c r="B29" t="s">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
-      <c r="B30" t="s">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
-      <c r="B31" t="s">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
-      <c r="B32" t="s">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="33" spans="2:2">
-      <c r="B33" t="s">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="34" spans="2:2">
-      <c r="B34" t="s">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B36" t="s">
         <v>36</v>
-      </c>
-    </row>
-    <row r="35" spans="2:2">
-      <c r="B35" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="36" spans="2:2">
-      <c r="B36" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>